<commit_message>
New datasets + baseline regression
</commit_message>
<xml_diff>
--- a/data/prs_categories.xlsx
+++ b/data/prs_categories.xlsx
@@ -10,7 +10,7 @@
     <sheet name="behavior" sheetId="1" r:id="rId1"/>
     <sheet name="lifestyle" sheetId="2" r:id="rId2"/>
     <sheet name="health" sheetId="3" r:id="rId3"/>
-    <sheet name="congenital" sheetId="4" r:id="rId4"/>
+    <sheet name="misc_long_term" sheetId="4" r:id="rId4"/>
     <sheet name="mental" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -613,7 +613,7 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>congenital</t>
+          <t>misc_long_term</t>
         </is>
       </c>
     </row>
@@ -708,7 +708,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -745,19 +745,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Ocular</t>
+          <t>Psychiatry</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
-        <is>
-          <t>Psychiatry</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
         <is>
           <t>Trauma</t>
         </is>

</xml_diff>